<commit_message>
fix: add modificaciones finales para la expo
</commit_message>
<xml_diff>
--- a/the_minion_game/docs/dsfem_resolucion_reto1.xlsx
+++ b/the_minion_game/docs/dsfem_resolucion_reto1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Skull\Documents\JUPYTER\DATASCIENCIEFEM\dsfem_datachallenge_monthly\the_minion_game\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7A9E3E-9B29-4E8F-A1C0-0CDBDE2598EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA076C02-B2F7-4944-B483-C1D2EBDF276F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="735" windowWidth="13215" windowHeight="15405" xr2:uid="{5BC759EF-AC07-4617-964F-D14EF8413DB2}"/>
+    <workbookView xWindow="8235" yWindow="195" windowWidth="13215" windowHeight="15405" xr2:uid="{5BC759EF-AC07-4617-964F-D14EF8413DB2}"/>
   </bookViews>
   <sheets>
     <sheet name="PASO N°1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>A,B,AB</t>
   </si>
   <si>
-    <t>A,B,C,AB,BC</t>
-  </si>
-  <si>
     <t>ABCD</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>=  6 -  5</t>
+  </si>
+  <si>
+    <t>A,B,C,AB,BC,ABC</t>
   </si>
 </sst>
 </file>
@@ -427,6 +427,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -439,31 +460,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DFEDEA-E7B9-4029-AF19-F8537EFE6BB3}">
   <dimension ref="B7:F14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,13 +807,13 @@
         <v>0</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -831,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -848,7 +848,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -859,73 +859,73 @@
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1">
         <v>6</v>
       </c>
-      <c r="E10" s="1">
-        <v>5</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1">
         <v>10</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1">
         <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1">
         <v>15</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -972,22 +972,22 @@
       <c r="I6" s="11"/>
     </row>
     <row r="7" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D7" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="31" t="s">
+      <c r="D7" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="26" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1020,27 +1020,27 @@
       <c r="I9" s="9"/>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="32" t="s">
+      <c r="K14" s="28" t="s">
         <v>30</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="K14" s="36" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.25">
@@ -1051,13 +1051,13 @@
         <v>2</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>2</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>2</v>
@@ -1076,66 +1076,66 @@
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="15"/>
-      <c r="J16" s="23">
+      <c r="J16" s="30">
         <v>5</v>
       </c>
-      <c r="K16" s="25" t="s">
-        <v>35</v>
+      <c r="K16" s="32" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="19"/>
       <c r="D17" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="25"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="32"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C18" s="19"/>
       <c r="D18" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="15"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="25"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="32"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C19" s="19"/>
       <c r="D19" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="15"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="25"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="32"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C20" s="20"/>
       <c r="D20" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="17"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="26"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="33"/>
       <c r="L20" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.25">
@@ -1146,7 +1146,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>2</v>
@@ -1167,40 +1167,40 @@
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="15"/>
-      <c r="J22" s="23">
+      <c r="J22" s="30">
         <v>3</v>
       </c>
-      <c r="K22" s="25" t="s">
-        <v>36</v>
+      <c r="K22" s="32" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C23" s="19"/>
       <c r="D23" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="15"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="25"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="32"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C24" s="20"/>
       <c r="D24" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
       <c r="I24" s="17"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="26"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="33"/>
       <c r="L24" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
@@ -1231,11 +1231,11 @@
       <c r="J26" s="20">
         <v>1</v>
       </c>
-      <c r="K26" s="27" t="s">
-        <v>37</v>
+      <c r="K26" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>